<commit_message>
A test complete run.
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8026D7C0-E154-45BA-A4FC-455A7E1695A4}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D6D0C6-EEE8-4F11-A1AC-FE73EA62D744}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>CvLAC</t>
   </si>
   <si>
-    <t>Adolfo</t>
-  </si>
-  <si>
-    <t>Alarcon Guzman</t>
-  </si>
-  <si>
     <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001545295</t>
   </si>
   <si>
@@ -59,7 +53,13 @@
     <t>Embus</t>
   </si>
   <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000218430</t>
+    <t>Juan Miguel David</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001458832</t>
+  </si>
+  <si>
+    <t>Becerra Tobar</t>
   </si>
 </sst>
 </file>
@@ -574,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,13 +606,13 @@
         <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>321</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -636,7 +636,7 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{B11CAD1C-7E9D-4E96-8B40-AA70F37FF48D}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{85F56D2F-86CF-418B-AB40-6D1C67C23E1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Apropiación insert was corrected to fill UAPABD.
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\CvLAC-Complete\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D6D0C6-EEE8-4F11-A1AC-FE73EA62D744}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -575,7 +574,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +602,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123</v>
+        <v>1024484682</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -617,7 +616,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>321</v>
+        <v>1032456871</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Final stage, commits were corrected.
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\CvLAC-Complete\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\CvLAC-Complete\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="CORREO">#REF!</definedName>
     <definedName name="Nombre">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Documento</t>
   </si>
@@ -59,13 +59,22 @@
   </si>
   <si>
     <t>Becerra Tobar</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000142522</t>
+  </si>
+  <si>
+    <t>Carlos Julio</t>
+  </si>
+  <si>
+    <t>Cortes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,6 +100,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -150,7 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -159,11 +176,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -190,7 +208,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{07834862-2E98-4B34-9FB5-A501111661BB}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -570,14 +588,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -618,7 +636,7 @@
       <c r="A3">
         <v>1032456871</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
@@ -628,16 +646,31 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:D1">
     <sortState ref="A2:D2">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{85F56D2F-86CF-418B-AB40-6D1C67C23E1D}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://www.google.com/url?q=http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh%3D0000142522&amp;sa=D&amp;source=hangouts&amp;ust=1521740785710000&amp;usg=AFQjCNGB77q4x9G4ftIe4x9qdZjq8byGLA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some changes on insert
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Documento</t>
   </si>
@@ -51,30 +51,12 @@
   <si>
     <t>Embus</t>
   </si>
-  <si>
-    <t>Juan Miguel David</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001458832</t>
-  </si>
-  <si>
-    <t>Becerra Tobar</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000142522</t>
-  </si>
-  <si>
-    <t>Carlos Julio</t>
-  </si>
-  <si>
-    <t>Cortes</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -92,22 +74,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -162,12 +128,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,11 +140,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
@@ -589,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,44 +583,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1024484682</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+        <v>1032456871</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1032456871</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>123</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -666,11 +601,7 @@
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2" display="https://www.google.com/url?q=http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh%3D0000142522&amp;sa=D&amp;source=hangouts&amp;ust=1521740785710000&amp;usg=AFQjCNGB77q4x9G4ftIe4x9qdZjq8byGLA"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final changes solving the ' issue and other little corrections.
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\CvLAC-Complete\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D908FF0-82DD-44D3-82EE-A52601F50E0A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Documento</t>
   </si>
@@ -42,20 +43,11 @@
   <si>
     <t>CvLAC</t>
   </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001545295</t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
-    <t>Embus</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,7 +124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,11 +132,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -171,7 +162,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -551,14 +542,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -581,26 +572,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1032456871</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:D1">
-    <sortState ref="A2:D2">
-      <sortCondition ref="D1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Resultados and Logs folder were added
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\CvLAC-Complete\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D908FF0-82DD-44D3-82EE-A52601F50E0A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Documento</t>
   </si>
@@ -42,12 +41,138 @@
   </si>
   <si>
     <t>CvLAC</t>
+  </si>
+  <si>
+    <t>Eliana</t>
+  </si>
+  <si>
+    <t>Lozano Romero</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001371417</t>
+  </si>
+  <si>
+    <t>Camilo Antonio</t>
+  </si>
+  <si>
+    <t>Monroy Peña</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001240633</t>
+  </si>
+  <si>
+    <t>Luis Miguel</t>
+  </si>
+  <si>
+    <t>Serrano Bermudez</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001353347</t>
+  </si>
+  <si>
+    <t>Gerson Andres</t>
+  </si>
+  <si>
+    <t>Rodriguez Rodriguez</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001421474</t>
+  </si>
+  <si>
+    <t>Edwin Alexander</t>
+  </si>
+  <si>
+    <t>Ramirez Perez</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001479088</t>
+  </si>
+  <si>
+    <t>Oscar Libardo</t>
+  </si>
+  <si>
+    <t>Lombana Charfuelan</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001413927</t>
+  </si>
+  <si>
+    <t>Alfonso</t>
+  </si>
+  <si>
+    <t>Martinez Andrade</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000013192</t>
+  </si>
+  <si>
+    <t>German Andres</t>
+  </si>
+  <si>
+    <t>Cabrera Rojas</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001468331</t>
+  </si>
+  <si>
+    <t>Jaime Leon</t>
+  </si>
+  <si>
+    <t>Aguilar Arias</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000266299</t>
+  </si>
+  <si>
+    <t>Luis Carlos</t>
+  </si>
+  <si>
+    <t>Belalcazar Ceron</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000249360</t>
+  </si>
+  <si>
+    <t>Jose Herney</t>
+  </si>
+  <si>
+    <t>Ramirez Franco</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000773093</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Jimenez Pizarro</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000177725</t>
+  </si>
+  <si>
+    <t>Marcelo Enrique</t>
+  </si>
+  <si>
+    <t>Riveros Rojas</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001447216</t>
+  </si>
+  <si>
+    <t>Armando</t>
+  </si>
+  <si>
+    <t>Espinosa Hernandez</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000105244</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -134,8 +259,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -162,7 +287,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -542,14 +667,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
@@ -572,8 +697,204 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1024496205</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1032363637</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1032389108</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1032419449</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1057581307</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1082104140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1121859744</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1136881212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>14894713</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>15813899</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>15920734</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>16737949</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>19136869</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>19187789</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Non ASCII characters were removed
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Documento</t>
   </si>
@@ -41,123 +41,6 @@
   </si>
   <si>
     <t>CvLAC</t>
-  </si>
-  <si>
-    <t>Eliana</t>
-  </si>
-  <si>
-    <t>Lozano Romero</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001371417</t>
-  </si>
-  <si>
-    <t>Camilo Antonio</t>
-  </si>
-  <si>
-    <t>Monroy Peña</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001240633</t>
-  </si>
-  <si>
-    <t>Luis Miguel</t>
-  </si>
-  <si>
-    <t>Serrano Bermudez</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001353347</t>
-  </si>
-  <si>
-    <t>Gerson Andres</t>
-  </si>
-  <si>
-    <t>Rodriguez Rodriguez</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001421474</t>
-  </si>
-  <si>
-    <t>Edwin Alexander</t>
-  </si>
-  <si>
-    <t>Ramirez Perez</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001479088</t>
-  </si>
-  <si>
-    <t>Oscar Libardo</t>
-  </si>
-  <si>
-    <t>Lombana Charfuelan</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001413927</t>
-  </si>
-  <si>
-    <t>Alfonso</t>
-  </si>
-  <si>
-    <t>Martinez Andrade</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000013192</t>
-  </si>
-  <si>
-    <t>German Andres</t>
-  </si>
-  <si>
-    <t>Cabrera Rojas</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001468331</t>
-  </si>
-  <si>
-    <t>Jaime Leon</t>
-  </si>
-  <si>
-    <t>Aguilar Arias</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000266299</t>
-  </si>
-  <si>
-    <t>Luis Carlos</t>
-  </si>
-  <si>
-    <t>Belalcazar Ceron</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000249360</t>
-  </si>
-  <si>
-    <t>Jose Herney</t>
-  </si>
-  <si>
-    <t>Ramirez Franco</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000773093</t>
-  </si>
-  <si>
-    <t>Rodrigo</t>
-  </si>
-  <si>
-    <t>Jimenez Pizarro</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000177725</t>
-  </si>
-  <si>
-    <t>Marcelo Enrique</t>
-  </si>
-  <si>
-    <t>Riveros Rojas</t>
-  </si>
-  <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001447216</t>
   </si>
   <si>
     <t>Armando</t>
@@ -668,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -699,7 +582,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1024496205</v>
+        <v>19187789</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -709,188 +592,6 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1032363637</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1032389108</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1032419449</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1057581307</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1082104140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1121859744</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1136881212</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>14894713</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>15813899</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>15920734</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>16737949</v>
-      </c>
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>19136869</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>19187789</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue with spanish characters was solved
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -43,13 +43,13 @@
     <t>CvLAC</t>
   </si>
   <si>
-    <t>Armando</t>
+    <t>Manuel</t>
   </si>
   <si>
-    <t>Espinosa Hernandez</t>
+    <t>Neira Embus</t>
   </si>
   <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000105244</t>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001545295</t>
   </si>
 </sst>
 </file>
@@ -132,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +140,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +583,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>19187789</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -590,7 +591,7 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Section 'Idiomas' was added to Results.
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10320" windowHeight="5670" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -74,6 +74,14 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -128,9 +136,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -140,9 +149,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
@@ -554,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -597,7 +607,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>